<commit_message>
update legend to DistStream and large-KDD99
</commit_message>
<xml_diff>
--- a/src/Data/ClusteringQuality/CluStream/Clustream-Cover-Normalized.xlsx
+++ b/src/Data/ClusteringQuality/CluStream/Clustream-Cover-Normalized.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kk/Documents/ISCAS/StreamingML/document/clustering/streamclustering/TestResult/pic/0509CMMNormalied/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kk/Repositories/PythonGraph/src/Data/ClusteringQuality/CluStream/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,11 +36,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ordered-CluStream</t>
+    <t>MOA=1.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MOA=1.0</t>
+    <t>DistStream-CluStream</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -468,23 +468,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Modify the clustering quality style of CluStream and DenStream
</commit_message>
<xml_diff>
--- a/src/Data/ClusteringQuality/CluStream/Clustream-Cover-Normalized.xlsx
+++ b/src/Data/ClusteringQuality/CluStream/Clustream-Cover-Normalized.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kk/Repositories/PythonGraph/src/Data/ClusteringQuality/CluStream/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31820" yWindow="2300" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,16 +27,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>unordered-CluStream</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MOA=1.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DistStream-CluStream</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unordered-CluStream</t>
   </si>
 </sst>
 </file>
@@ -52,14 +46,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -68,7 +62,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -77,7 +71,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -144,17 +138,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -212,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -264,7 +258,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -458,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -469,31 +463,31 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -507,7 +501,7 @@
         <v>0.54684617499999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -521,7 +515,7 @@
         <v>0.97275196100000005</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>30</v>
       </c>
@@ -535,7 +529,7 @@
         <v>0.98013884299999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>40</v>
       </c>
@@ -549,7 +543,7 @@
         <v>0.98138059600000005</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>50</v>
       </c>
@@ -563,7 +557,7 @@
         <v>0.99893239300000003</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>60</v>
       </c>
@@ -577,7 +571,7 @@
         <v>0.99608416099999997</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>70</v>
       </c>
@@ -591,7 +585,7 @@
         <v>0.97629627900000004</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>80</v>
       </c>
@@ -605,7 +599,7 @@
         <v>0.96142734200000002</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>90</v>
       </c>
@@ -619,7 +613,7 @@
         <v>0.997908868</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>100</v>
       </c>
@@ -633,7 +627,7 @@
         <v>0.97966569599999997</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>110</v>
       </c>
@@ -647,7 +641,7 @@
         <v>0.99599705299999997</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>120</v>
       </c>
@@ -661,7 +655,7 @@
         <v>0.95112542099999997</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>130</v>
       </c>
@@ -675,7 +669,7 @@
         <v>1.0046923000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>140</v>
       </c>
@@ -689,7 +683,7 @@
         <v>1.011897201</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>150</v>
       </c>
@@ -703,7 +697,7 @@
         <v>1.005556975</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>160</v>
       </c>
@@ -717,7 +711,7 @@
         <v>1.015158446</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>170</v>
       </c>
@@ -731,7 +725,7 @@
         <v>1.0002961319999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>180</v>
       </c>
@@ -745,7 +739,7 @@
         <v>0.96287174900000005</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>190</v>
       </c>
@@ -759,7 +753,7 @@
         <v>0.96433972999999995</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>200</v>
       </c>
@@ -773,7 +767,7 @@
         <v>1.006573978</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>210</v>
       </c>
@@ -787,7 +781,7 @@
         <v>0.38826962500000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>220</v>
       </c>
@@ -801,7 +795,7 @@
         <v>0.86999880200000002</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>230</v>
       </c>
@@ -815,7 +809,7 @@
         <v>0.77869608899999998</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>240</v>
       </c>
@@ -829,7 +823,7 @@
         <v>0.79232562799999995</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>250</v>
       </c>
@@ -843,7 +837,7 @@
         <v>0.79790190100000002</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>260</v>
       </c>
@@ -857,7 +851,7 @@
         <v>0.72159657899999996</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>270</v>
       </c>
@@ -871,7 +865,7 @@
         <v>0.70811856100000004</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>280</v>
       </c>
@@ -885,7 +879,7 @@
         <v>0.82474174899999997</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>290</v>
       </c>
@@ -899,7 +893,7 @@
         <v>0.75068127500000004</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>300</v>
       </c>
@@ -913,7 +907,7 @@
         <v>0.87517391300000003</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>310</v>
       </c>
@@ -927,7 +921,7 @@
         <v>0.86472713199999995</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>320</v>
       </c>
@@ -941,7 +935,7 @@
         <v>0.84672341200000001</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>330</v>
       </c>
@@ -955,7 +949,7 @@
         <v>0.88752284699999995</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>340</v>
       </c>
@@ -969,7 +963,7 @@
         <v>0.87927025999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>350</v>
       </c>
@@ -983,7 +977,7 @@
         <v>0.88712146000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>360</v>
       </c>
@@ -997,7 +991,7 @@
         <v>0.90838797800000004</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>370</v>
       </c>
@@ -1011,7 +1005,7 @@
         <v>0.94092230700000001</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>380</v>
       </c>
@@ -1025,7 +1019,7 @@
         <v>0.96534773699999998</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>390</v>
       </c>
@@ -1039,7 +1033,7 @@
         <v>0.92209730999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>400</v>
       </c>
@@ -1053,7 +1047,7 @@
         <v>0.93463450800000003</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>410</v>
       </c>
@@ -1067,7 +1061,7 @@
         <v>0.92289498999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>420</v>
       </c>
@@ -1081,7 +1075,7 @@
         <v>0.950186156</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>430</v>
       </c>
@@ -1095,7 +1089,7 @@
         <v>0.89850663399999997</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>440</v>
       </c>
@@ -1109,7 +1103,7 @@
         <v>0.940511769</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>450</v>
       </c>
@@ -1123,7 +1117,7 @@
         <v>0.97696694799999995</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>460</v>
       </c>
@@ -1137,7 +1131,7 @@
         <v>0.99403706999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>470</v>
       </c>
@@ -1151,7 +1145,7 @@
         <v>0.94424710999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>480</v>
       </c>
@@ -1165,7 +1159,7 @@
         <v>0.93889239499999999</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>490</v>
       </c>
@@ -1179,7 +1173,7 @@
         <v>0.892065522</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>500</v>
       </c>
@@ -1193,7 +1187,7 @@
         <v>0.94878875100000004</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="1">
         <v>510</v>
       </c>
@@ -1207,7 +1201,7 @@
         <v>1.001160345</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="1">
         <v>520</v>
       </c>
@@ -1221,7 +1215,7 @@
         <v>0.98719761100000003</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="1">
         <v>530</v>
       </c>
@@ -1235,7 +1229,7 @@
         <v>0.89289277300000003</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="1">
         <v>540</v>
       </c>
@@ -1249,7 +1243,7 @@
         <v>0.941425281</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="1">
         <v>550</v>
       </c>
@@ -1263,7 +1257,7 @@
         <v>0.95644491499999995</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="1">
         <v>560</v>
       </c>
@@ -1277,7 +1271,7 @@
         <v>0.421278718</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" s="1">
         <v>570</v>
       </c>
@@ -1291,7 +1285,7 @@
         <v>0.90603783100000002</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" s="1">
         <v>580</v>
       </c>
@@ -1308,5 +1302,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>